<commit_message>
added some code enhancements
</commit_message>
<xml_diff>
--- a/Excel reports/clb_raw_dataset.xlsx
+++ b/Excel reports/clb_raw_dataset.xlsx
@@ -493,7 +493,7 @@
         <v>40.09000015258789</v>
       </c>
       <c r="F2" t="n">
-        <v>39.65832901000977</v>
+        <v>39.6583251953125</v>
       </c>
       <c r="G2" t="n">
         <v>6842800</v>
@@ -516,7 +516,7 @@
         <v>40.22999954223633</v>
       </c>
       <c r="F3" t="n">
-        <v>39.79682159423828</v>
+        <v>39.79681777954102</v>
       </c>
       <c r="G3" t="n">
         <v>3646800</v>
@@ -539,7 +539,7 @@
         <v>39.83000183105469</v>
       </c>
       <c r="F4" t="n">
-        <v>39.4011344909668</v>
+        <v>39.40112686157227</v>
       </c>
       <c r="G4" t="n">
         <v>2796400</v>
@@ -562,7 +562,7 @@
         <v>37.86999893188477</v>
       </c>
       <c r="F5" t="n">
-        <v>37.46223068237305</v>
+        <v>37.46223831176758</v>
       </c>
       <c r="G5" t="n">
         <v>2137600</v>
@@ -642,7 +642,7 @@
         <v>33.75</v>
       </c>
       <c r="F9" t="n">
-        <v>33.60166168212891</v>
+        <v>33.60165405273438</v>
       </c>
       <c r="G9" t="n">
         <v>3580800</v>
@@ -665,7 +665,7 @@
         <v>31.20000076293945</v>
       </c>
       <c r="F10" t="n">
-        <v>31.0628662109375</v>
+        <v>31.06286811828613</v>
       </c>
       <c r="G10" t="n">
         <v>2383400</v>
@@ -688,7 +688,7 @@
         <v>26.84000015258789</v>
       </c>
       <c r="F11" t="n">
-        <v>26.7220287322998</v>
+        <v>26.7220344543457</v>
       </c>
       <c r="G11" t="n">
         <v>6064900</v>
@@ -711,7 +711,7 @@
         <v>23.84000015258789</v>
       </c>
       <c r="F12" t="n">
-        <v>23.73521423339844</v>
+        <v>23.73521614074707</v>
       </c>
       <c r="G12" t="n">
         <v>7395600</v>
@@ -734,7 +734,7 @@
         <v>8.489999771118164</v>
       </c>
       <c r="F13" t="n">
-        <v>8.452683448791504</v>
+        <v>8.45268440246582</v>
       </c>
       <c r="G13" t="n">
         <v>21662300</v>
@@ -757,7 +757,7 @@
         <v>9.949999809265137</v>
       </c>
       <c r="F14" t="n">
-        <v>9.906266212463379</v>
+        <v>9.906265258789062</v>
       </c>
       <c r="G14" t="n">
         <v>18552500</v>
@@ -803,7 +803,7 @@
         <v>9.899999618530273</v>
       </c>
       <c r="F16" t="n">
-        <v>9.856486320495605</v>
+        <v>9.856485366821289</v>
       </c>
       <c r="G16" t="n">
         <v>8158700</v>
@@ -826,7 +826,7 @@
         <v>11.67000007629395</v>
       </c>
       <c r="F17" t="n">
-        <v>11.61870765686035</v>
+        <v>11.61870670318604</v>
       </c>
       <c r="G17" t="n">
         <v>6303600</v>
@@ -849,7 +849,7 @@
         <v>11.75</v>
       </c>
       <c r="F18" t="n">
-        <v>11.69835472106934</v>
+        <v>11.69835662841797</v>
       </c>
       <c r="G18" t="n">
         <v>6716700</v>
@@ -872,7 +872,7 @@
         <v>14.96000003814697</v>
       </c>
       <c r="F19" t="n">
-        <v>14.89424705505371</v>
+        <v>14.89424514770508</v>
       </c>
       <c r="G19" t="n">
         <v>9980100</v>
@@ -952,7 +952,7 @@
         <v>18.06999969482422</v>
       </c>
       <c r="F23" t="n">
-        <v>18.00143051147461</v>
+        <v>18.00142669677734</v>
       </c>
       <c r="G23" t="n">
         <v>4177900</v>
@@ -998,7 +998,7 @@
         <v>20.21999931335449</v>
       </c>
       <c r="F25" t="n">
-        <v>20.14326858520508</v>
+        <v>20.14326667785645</v>
       </c>
       <c r="G25" t="n">
         <v>3887800</v>
@@ -1021,7 +1021,7 @@
         <v>26.86000061035156</v>
       </c>
       <c r="F26" t="n">
-        <v>26.7580738067627</v>
+        <v>26.75807189941406</v>
       </c>
       <c r="G26" t="n">
         <v>4851600</v>
@@ -1044,7 +1044,7 @@
         <v>23.8700008392334</v>
       </c>
       <c r="F27" t="n">
-        <v>23.77941703796387</v>
+        <v>23.77942085266113</v>
       </c>
       <c r="G27" t="n">
         <v>5098000</v>
@@ -1090,7 +1090,7 @@
         <v>19.65999984741211</v>
       </c>
       <c r="F29" t="n">
-        <v>19.58539390563965</v>
+        <v>19.58539199829102</v>
       </c>
       <c r="G29" t="n">
         <v>4940700</v>
@@ -1182,7 +1182,7 @@
         <v>23.73999977111816</v>
       </c>
       <c r="F33" t="n">
-        <v>23.6499080657959</v>
+        <v>23.64990997314453</v>
       </c>
       <c r="G33" t="n">
         <v>5157800</v>
@@ -1216,7 +1216,7 @@
         <v>21.32999992370605</v>
       </c>
       <c r="F35" t="n">
-        <v>21.25806045532227</v>
+        <v>21.2580623626709</v>
       </c>
       <c r="G35" t="n">
         <v>2854100</v>
@@ -1262,7 +1262,7 @@
         <v>24.52000045776367</v>
       </c>
       <c r="F37" t="n">
-        <v>24.43729972839355</v>
+        <v>24.43730163574219</v>
       </c>
       <c r="G37" t="n">
         <v>2041600</v>
@@ -1285,7 +1285,7 @@
         <v>22.3799991607666</v>
       </c>
       <c r="F38" t="n">
-        <v>22.30451774597168</v>
+        <v>22.30451965332031</v>
       </c>
       <c r="G38" t="n">
         <v>1945900</v>
@@ -1331,7 +1331,7 @@
         <v>20.86000061035156</v>
       </c>
       <c r="F40" t="n">
-        <v>20.78964805603027</v>
+        <v>20.78964424133301</v>
       </c>
       <c r="G40" t="n">
         <v>1929000</v>
@@ -1354,7 +1354,7 @@
         <v>17.6299991607666</v>
       </c>
       <c r="F41" t="n">
-        <v>17.57054328918457</v>
+        <v>17.5705394744873</v>
       </c>
       <c r="G41" t="n">
         <v>1619400</v>
@@ -1492,7 +1492,7 @@
         <v>15.35000038146973</v>
       </c>
       <c r="F47" t="n">
-        <v>15.2982292175293</v>
+        <v>15.29822826385498</v>
       </c>
       <c r="G47" t="n">
         <v>2933800</v>
@@ -1526,7 +1526,7 @@
         <v>14.44999980926514</v>
       </c>
       <c r="F49" t="n">
-        <v>14.4108829498291</v>
+        <v>14.41088390350342</v>
       </c>
       <c r="G49" t="n">
         <v>2461800</v>
@@ -1549,7 +1549,7 @@
         <v>15.21000003814697</v>
       </c>
       <c r="F50" t="n">
-        <v>15.16882705688477</v>
+        <v>15.16882801055908</v>
       </c>
       <c r="G50" t="n">
         <v>2323100</v>
@@ -1572,7 +1572,7 @@
         <v>18.3799991607666</v>
       </c>
       <c r="F51" t="n">
-        <v>18.33024597167969</v>
+        <v>18.33024787902832</v>
       </c>
       <c r="G51" t="n">
         <v>2323300</v>
@@ -1595,7 +1595,7 @@
         <v>20.19000053405762</v>
       </c>
       <c r="F52" t="n">
-        <v>20.13534736633301</v>
+        <v>20.13534927368164</v>
       </c>
       <c r="G52" t="n">
         <v>2081900</v>
@@ -1710,7 +1710,7 @@
         <v>26.13999938964844</v>
       </c>
       <c r="F57" t="n">
-        <v>26.06923866271973</v>
+        <v>26.06924057006836</v>
       </c>
       <c r="G57" t="n">
         <v>2381700</v>
@@ -1733,7 +1733,7 @@
         <v>26.51000022888184</v>
       </c>
       <c r="F58" t="n">
-        <v>26.4382381439209</v>
+        <v>26.43824005126953</v>
       </c>
       <c r="G58" t="n">
         <v>1657300</v>
@@ -1756,7 +1756,7 @@
         <v>30.97999954223633</v>
       </c>
       <c r="F59" t="n">
-        <v>30.89613914489746</v>
+        <v>30.89613723754883</v>
       </c>
       <c r="G59" t="n">
         <v>2476300</v>
@@ -1836,7 +1836,7 @@
         <v>32.97999954223633</v>
       </c>
       <c r="F63" t="n">
-        <v>32.90045166015625</v>
+        <v>32.90044784545898</v>
       </c>
       <c r="G63" t="n">
         <v>3208000</v>
@@ -1859,7 +1859,7 @@
         <v>35.7599983215332</v>
       </c>
       <c r="F64" t="n">
-        <v>35.67374420166016</v>
+        <v>35.67374038696289</v>
       </c>
       <c r="G64" t="n">
         <v>1670400</v>
@@ -1882,7 +1882,7 @@
         <v>34.72999954223633</v>
       </c>
       <c r="F65" t="n">
-        <v>34.6462287902832</v>
+        <v>34.64622497558594</v>
       </c>
       <c r="G65" t="n">
         <v>1670100</v>
@@ -1905,7 +1905,7 @@
         <v>35.08000183105469</v>
       </c>
       <c r="F66" t="n">
-        <v>34.99538040161133</v>
+        <v>34.99538803100586</v>
       </c>
       <c r="G66" t="n">
         <v>1516700</v>
@@ -1928,7 +1928,7 @@
         <v>35.54000091552734</v>
       </c>
       <c r="F67" t="n">
-        <v>35.45427703857422</v>
+        <v>35.45427322387695</v>
       </c>
       <c r="G67" t="n">
         <v>2603000</v>
@@ -1974,7 +1974,7 @@
         <v>37.45999908447266</v>
       </c>
       <c r="F69" t="n">
-        <v>37.3696403503418</v>
+        <v>37.36964416503906</v>
       </c>
       <c r="G69" t="n">
         <v>2931700</v>
@@ -2066,7 +2066,7 @@
         <v>27.23999977111816</v>
       </c>
       <c r="F73" t="n">
-        <v>27.17429161071777</v>
+        <v>27.17429351806641</v>
       </c>
       <c r="G73" t="n">
         <v>1666100</v>
@@ -2089,7 +2089,7 @@
         <v>27.53000068664551</v>
       </c>
       <c r="F74" t="n">
-        <v>27.46359252929688</v>
+        <v>27.46359634399414</v>
       </c>
       <c r="G74" t="n">
         <v>1764700</v>
@@ -2135,7 +2135,7 @@
         <v>28.18000030517578</v>
       </c>
       <c r="F76" t="n">
-        <v>28.11202430725098</v>
+        <v>28.11202621459961</v>
       </c>
       <c r="G76" t="n">
         <v>1589200</v>
@@ -2169,7 +2169,7 @@
         <v>33.81000137329102</v>
       </c>
       <c r="F78" t="n">
-        <v>33.73976135253906</v>
+        <v>33.73976516723633</v>
       </c>
       <c r="G78" t="n">
         <v>2114000</v>
@@ -2215,7 +2215,7 @@
         <v>37.45000076293945</v>
       </c>
       <c r="F80" t="n">
-        <v>37.3722038269043</v>
+        <v>37.37220001220703</v>
       </c>
       <c r="G80" t="n">
         <v>3756700</v>
@@ -2261,7 +2261,7 @@
         <v>47.56000137329102</v>
       </c>
       <c r="F82" t="n">
-        <v>47.46120071411133</v>
+        <v>47.46120452880859</v>
       </c>
       <c r="G82" t="n">
         <v>3090400</v>
@@ -2284,7 +2284,7 @@
         <v>47.81000137329102</v>
       </c>
       <c r="F83" t="n">
-        <v>47.71068572998047</v>
+        <v>47.71067810058594</v>
       </c>
       <c r="G83" t="n">
         <v>1862300</v>
@@ -2307,7 +2307,7 @@
         <v>41.34999847412109</v>
       </c>
       <c r="F84" t="n">
-        <v>41.26410293579102</v>
+        <v>41.26409912109375</v>
       </c>
       <c r="G84" t="n">
         <v>3097400</v>
@@ -2330,7 +2330,7 @@
         <v>42.11000061035156</v>
       </c>
       <c r="F85" t="n">
-        <v>42.02252197265625</v>
+        <v>42.02252578735352</v>
       </c>
       <c r="G85" t="n">
         <v>2550300</v>
@@ -2353,7 +2353,7 @@
         <v>38.7599983215332</v>
       </c>
       <c r="F86" t="n">
-        <v>38.67947387695312</v>
+        <v>38.67948532104492</v>
       </c>
       <c r="G86" t="n">
         <v>2483600</v>
@@ -2376,7 +2376,7 @@
         <v>36.16999816894531</v>
       </c>
       <c r="F87" t="n">
-        <v>36.0948600769043</v>
+        <v>36.09485626220703</v>
       </c>
       <c r="G87" t="n">
         <v>3135100</v>
@@ -2399,7 +2399,7 @@
         <v>33.79000091552734</v>
       </c>
       <c r="F88" t="n">
-        <v>33.71980285644531</v>
+        <v>33.71980667114258</v>
       </c>
       <c r="G88" t="n">
         <v>2492500</v>
@@ -2422,7 +2422,7 @@
         <v>33.09000015258789</v>
       </c>
       <c r="F89" t="n">
-        <v>33.02126312255859</v>
+        <v>33.02125549316406</v>
       </c>
       <c r="G89" t="n">
         <v>1703400</v>
@@ -2468,7 +2468,7 @@
         <v>30.34000015258789</v>
       </c>
       <c r="F91" t="n">
-        <v>30.2769718170166</v>
+        <v>30.27697372436523</v>
       </c>
       <c r="G91" t="n">
         <v>2448100</v>
@@ -2502,7 +2502,7 @@
         <v>28.53000068664551</v>
       </c>
       <c r="F93" t="n">
-        <v>28.48008346557617</v>
+        <v>28.4800853729248</v>
       </c>
       <c r="G93" t="n">
         <v>2586200</v>
@@ -2548,7 +2548,7 @@
         <v>28.93000030517578</v>
       </c>
       <c r="F95" t="n">
-        <v>28.87938499450684</v>
+        <v>28.8793830871582</v>
       </c>
       <c r="G95" t="n">
         <v>2421800</v>
@@ -2594,7 +2594,7 @@
         <v>27.81999969482422</v>
       </c>
       <c r="F97" t="n">
-        <v>27.77132606506348</v>
+        <v>27.77132415771484</v>
       </c>
       <c r="G97" t="n">
         <v>1793400</v>
@@ -2640,7 +2640,7 @@
         <v>27.19000053405762</v>
       </c>
       <c r="F99" t="n">
-        <v>27.14242553710938</v>
+        <v>27.14242744445801</v>
       </c>
       <c r="G99" t="n">
         <v>3205000</v>
@@ -2709,7 +2709,7 @@
         <v>31.54000091552734</v>
       </c>
       <c r="F102" t="n">
-        <v>31.48481941223145</v>
+        <v>31.48481559753418</v>
       </c>
       <c r="G102" t="n">
         <v>1670000</v>
@@ -2732,7 +2732,7 @@
         <v>28.22999954223633</v>
       </c>
       <c r="F103" t="n">
-        <v>28.18060874938965</v>
+        <v>28.18060684204102</v>
       </c>
       <c r="G103" t="n">
         <v>2161300</v>
@@ -2858,7 +2858,7 @@
         <v>24.13999938964844</v>
       </c>
       <c r="F109" t="n">
-        <v>24.10663414001465</v>
+        <v>24.10663223266602</v>
       </c>
       <c r="G109" t="n">
         <v>1581200</v>
@@ -2927,7 +2927,7 @@
         <v>22.43000030517578</v>
       </c>
       <c r="F112" t="n">
-        <v>22.39899826049805</v>
+        <v>22.39899635314941</v>
       </c>
       <c r="G112" t="n">
         <v>2549300</v>
@@ -2950,7 +2950,7 @@
         <v>23.25</v>
       </c>
       <c r="F113" t="n">
-        <v>23.21786499023438</v>
+        <v>23.21786308288574</v>
       </c>
       <c r="G113" t="n">
         <v>1012300</v>
@@ -2973,7 +2973,7 @@
         <v>22.30999946594238</v>
       </c>
       <c r="F114" t="n">
-        <v>22.27916145324707</v>
+        <v>22.2791633605957</v>
       </c>
       <c r="G114" t="n">
         <v>1336400</v>
@@ -3019,7 +3019,7 @@
         <v>27.35000038146973</v>
       </c>
       <c r="F116" t="n">
-        <v>27.31219673156738</v>
+        <v>27.31219863891602</v>
       </c>
       <c r="G116" t="n">
         <v>1510600</v>
@@ -3111,7 +3111,7 @@
         <v>28.13999938964844</v>
       </c>
       <c r="F120" t="n">
-        <v>28.10110473632812</v>
+        <v>28.10110282897949</v>
       </c>
       <c r="G120" t="n">
         <v>3067300</v>
@@ -3191,7 +3191,7 @@
         <v>27.13999938964844</v>
       </c>
       <c r="F124" t="n">
-        <v>27.11292457580566</v>
+        <v>27.11292266845703</v>
       </c>
       <c r="G124" t="n">
         <v>3140400</v>
@@ -3237,7 +3237,7 @@
         <v>29</v>
       </c>
       <c r="F126" t="n">
-        <v>28.97106742858887</v>
+        <v>28.9710693359375</v>
       </c>
       <c r="G126" t="n">
         <v>4601700</v>

</xml_diff>

<commit_message>
sentiment analysis under construction
</commit_message>
<xml_diff>
--- a/Excel reports/clb_raw_dataset.xlsx
+++ b/Excel reports/clb_raw_dataset.xlsx
@@ -493,7 +493,7 @@
         <v>40.09000015258789</v>
       </c>
       <c r="F2" t="n">
-        <v>39.6583251953125</v>
+        <v>39.65832901000977</v>
       </c>
       <c r="G2" t="n">
         <v>6842800</v>
@@ -516,7 +516,7 @@
         <v>40.22999954223633</v>
       </c>
       <c r="F3" t="n">
-        <v>39.79681777954102</v>
+        <v>39.79682159423828</v>
       </c>
       <c r="G3" t="n">
         <v>3646800</v>
@@ -539,7 +539,7 @@
         <v>39.83000183105469</v>
       </c>
       <c r="F4" t="n">
-        <v>39.4011344909668</v>
+        <v>39.40113067626953</v>
       </c>
       <c r="G4" t="n">
         <v>2796400</v>
@@ -619,7 +619,7 @@
         <v>34.65999984741211</v>
       </c>
       <c r="F8" t="n">
-        <v>34.50765228271484</v>
+        <v>34.50765991210938</v>
       </c>
       <c r="G8" t="n">
         <v>3334900</v>
@@ -642,7 +642,7 @@
         <v>33.75</v>
       </c>
       <c r="F9" t="n">
-        <v>33.60165786743164</v>
+        <v>33.60165405273438</v>
       </c>
       <c r="G9" t="n">
         <v>3580800</v>
@@ -665,7 +665,7 @@
         <v>31.20000076293945</v>
       </c>
       <c r="F10" t="n">
-        <v>31.06286811828613</v>
+        <v>31.0628662109375</v>
       </c>
       <c r="G10" t="n">
         <v>2383400</v>
@@ -688,7 +688,7 @@
         <v>26.84000015258789</v>
       </c>
       <c r="F11" t="n">
-        <v>26.72203063964844</v>
+        <v>26.72202682495117</v>
       </c>
       <c r="G11" t="n">
         <v>6064900</v>
@@ -757,7 +757,7 @@
         <v>9.949999809265137</v>
       </c>
       <c r="F14" t="n">
-        <v>9.906266212463379</v>
+        <v>9.906267166137695</v>
       </c>
       <c r="G14" t="n">
         <v>18552500</v>
@@ -780,7 +780,7 @@
         <v>9.75</v>
       </c>
       <c r="F15" t="n">
-        <v>9.707144737243652</v>
+        <v>9.707145690917969</v>
       </c>
       <c r="G15" t="n">
         <v>7932000</v>
@@ -918,7 +918,7 @@
         <v>18.95000076293945</v>
       </c>
       <c r="F21" t="n">
-        <v>18.8667106628418</v>
+        <v>18.86670684814453</v>
       </c>
       <c r="G21" t="n">
         <v>5843200</v>
@@ -952,7 +952,7 @@
         <v>18.06999969482422</v>
       </c>
       <c r="F23" t="n">
-        <v>18.00142478942871</v>
+        <v>18.00142669677734</v>
       </c>
       <c r="G23" t="n">
         <v>4177900</v>
@@ -975,7 +975,7 @@
         <v>19.63999938964844</v>
       </c>
       <c r="F24" t="n">
-        <v>19.56546974182129</v>
+        <v>19.56546783447266</v>
       </c>
       <c r="G24" t="n">
         <v>3474500</v>
@@ -1113,7 +1113,7 @@
         <v>21.27000045776367</v>
       </c>
       <c r="F30" t="n">
-        <v>21.18928527832031</v>
+        <v>21.18928337097168</v>
       </c>
       <c r="G30" t="n">
         <v>2789600</v>
@@ -1136,7 +1136,7 @@
         <v>20.78000068664551</v>
       </c>
       <c r="F31" t="n">
-        <v>20.70114517211914</v>
+        <v>20.70114326477051</v>
       </c>
       <c r="G31" t="n">
         <v>3749300</v>
@@ -1159,7 +1159,7 @@
         <v>20.29999923706055</v>
       </c>
       <c r="F32" t="n">
-        <v>20.22296333312988</v>
+        <v>20.22296142578125</v>
       </c>
       <c r="G32" t="n">
         <v>3565800</v>
@@ -1182,7 +1182,7 @@
         <v>23.73999977111816</v>
       </c>
       <c r="F33" t="n">
-        <v>23.6499080657959</v>
+        <v>23.64990997314453</v>
       </c>
       <c r="G33" t="n">
         <v>5157800</v>
@@ -1216,7 +1216,7 @@
         <v>21.32999992370605</v>
       </c>
       <c r="F35" t="n">
-        <v>21.25805854797363</v>
+        <v>21.25806045532227</v>
       </c>
       <c r="G35" t="n">
         <v>2854100</v>
@@ -1262,7 +1262,7 @@
         <v>24.52000045776367</v>
       </c>
       <c r="F37" t="n">
-        <v>24.43730163574219</v>
+        <v>24.43729972839355</v>
       </c>
       <c r="G37" t="n">
         <v>2041600</v>
@@ -1285,7 +1285,7 @@
         <v>22.3799991607666</v>
       </c>
       <c r="F38" t="n">
-        <v>22.30451965332031</v>
+        <v>22.30451583862305</v>
       </c>
       <c r="G38" t="n">
         <v>1945900</v>
@@ -1331,7 +1331,7 @@
         <v>20.86000061035156</v>
       </c>
       <c r="F40" t="n">
-        <v>20.78964805603027</v>
+        <v>20.78964424133301</v>
       </c>
       <c r="G40" t="n">
         <v>1929000</v>
@@ -1400,7 +1400,7 @@
         <v>15.53999996185303</v>
       </c>
       <c r="F43" t="n">
-        <v>15.48758792877197</v>
+        <v>15.48758888244629</v>
       </c>
       <c r="G43" t="n">
         <v>2766500</v>
@@ -1423,7 +1423,7 @@
         <v>14.88000011444092</v>
       </c>
       <c r="F44" t="n">
-        <v>14.82981491088867</v>
+        <v>14.82981395721436</v>
       </c>
       <c r="G44" t="n">
         <v>3836300</v>
@@ -1446,7 +1446,7 @@
         <v>16.30999946594238</v>
       </c>
       <c r="F45" t="n">
-        <v>16.2549934387207</v>
+        <v>16.25498962402344</v>
       </c>
       <c r="G45" t="n">
         <v>2376800</v>
@@ -1492,7 +1492,7 @@
         <v>15.35000038146973</v>
       </c>
       <c r="F47" t="n">
-        <v>15.2982292175293</v>
+        <v>15.29823017120361</v>
       </c>
       <c r="G47" t="n">
         <v>2933800</v>
@@ -1526,7 +1526,7 @@
         <v>14.44999980926514</v>
       </c>
       <c r="F49" t="n">
-        <v>14.41088390350342</v>
+        <v>14.41088485717773</v>
       </c>
       <c r="G49" t="n">
         <v>2461800</v>
@@ -1572,7 +1572,7 @@
         <v>18.3799991607666</v>
       </c>
       <c r="F51" t="n">
-        <v>18.33024597167969</v>
+        <v>18.33024787902832</v>
       </c>
       <c r="G51" t="n">
         <v>2323300</v>
@@ -1595,7 +1595,7 @@
         <v>20.19000053405762</v>
       </c>
       <c r="F52" t="n">
-        <v>20.13534545898438</v>
+        <v>20.13534736633301</v>
       </c>
       <c r="G52" t="n">
         <v>2081900</v>
@@ -1618,7 +1618,7 @@
         <v>24.09000015258789</v>
       </c>
       <c r="F53" t="n">
-        <v>24.0247917175293</v>
+        <v>24.02478981018066</v>
       </c>
       <c r="G53" t="n">
         <v>2051500</v>
@@ -1641,7 +1641,7 @@
         <v>26.67000007629395</v>
       </c>
       <c r="F54" t="n">
-        <v>26.59780693054199</v>
+        <v>26.59780502319336</v>
       </c>
       <c r="G54" t="n">
         <v>2229800</v>
@@ -1710,7 +1710,7 @@
         <v>26.13999938964844</v>
       </c>
       <c r="F57" t="n">
-        <v>26.06923866271973</v>
+        <v>26.06924057006836</v>
       </c>
       <c r="G57" t="n">
         <v>2381700</v>
@@ -1733,7 +1733,7 @@
         <v>26.51000022888184</v>
       </c>
       <c r="F58" t="n">
-        <v>26.43824005126953</v>
+        <v>26.43824195861816</v>
       </c>
       <c r="G58" t="n">
         <v>1657300</v>
@@ -1779,7 +1779,7 @@
         <v>33.75</v>
       </c>
       <c r="F60" t="n">
-        <v>33.65864181518555</v>
+        <v>33.65863800048828</v>
       </c>
       <c r="G60" t="n">
         <v>2429600</v>
@@ -1802,7 +1802,7 @@
         <v>35.36000061035156</v>
       </c>
       <c r="F61" t="n">
-        <v>35.2642822265625</v>
+        <v>35.26428604125977</v>
       </c>
       <c r="G61" t="n">
         <v>1654600</v>
@@ -1859,7 +1859,7 @@
         <v>35.7599983215332</v>
       </c>
       <c r="F64" t="n">
-        <v>35.67374801635742</v>
+        <v>35.67374420166016</v>
       </c>
       <c r="G64" t="n">
         <v>1670400</v>
@@ -1882,7 +1882,7 @@
         <v>34.72999954223633</v>
       </c>
       <c r="F65" t="n">
-        <v>34.64622116088867</v>
+        <v>34.6462287902832</v>
       </c>
       <c r="G65" t="n">
         <v>1670100</v>
@@ -1928,7 +1928,7 @@
         <v>35.54000091552734</v>
       </c>
       <c r="F67" t="n">
-        <v>35.45427322387695</v>
+        <v>35.45427703857422</v>
       </c>
       <c r="G67" t="n">
         <v>2603000</v>
@@ -1974,7 +1974,7 @@
         <v>37.45999908447266</v>
       </c>
       <c r="F69" t="n">
-        <v>37.3696403503418</v>
+        <v>37.36963653564453</v>
       </c>
       <c r="G69" t="n">
         <v>2931700</v>
@@ -1997,7 +1997,7 @@
         <v>32.81999969482422</v>
       </c>
       <c r="F70" t="n">
-        <v>32.74082946777344</v>
+        <v>32.74083709716797</v>
       </c>
       <c r="G70" t="n">
         <v>3491200</v>
@@ -2020,7 +2020,7 @@
         <v>30.65999984741211</v>
       </c>
       <c r="F71" t="n">
-        <v>30.5860424041748</v>
+        <v>30.58604621887207</v>
       </c>
       <c r="G71" t="n">
         <v>2163100</v>
@@ -2043,7 +2043,7 @@
         <v>30.10000038146973</v>
       </c>
       <c r="F72" t="n">
-        <v>30.02739715576172</v>
+        <v>30.02739524841309</v>
       </c>
       <c r="G72" t="n">
         <v>1269300</v>
@@ -2089,7 +2089,7 @@
         <v>27.53000068664551</v>
       </c>
       <c r="F74" t="n">
-        <v>27.46359634399414</v>
+        <v>27.46359443664551</v>
       </c>
       <c r="G74" t="n">
         <v>1764700</v>
@@ -2135,7 +2135,7 @@
         <v>28.18000030517578</v>
       </c>
       <c r="F76" t="n">
-        <v>28.11202812194824</v>
+        <v>28.11202621459961</v>
       </c>
       <c r="G76" t="n">
         <v>1589200</v>
@@ -2169,7 +2169,7 @@
         <v>33.81000137329102</v>
       </c>
       <c r="F78" t="n">
-        <v>33.73976516723633</v>
+        <v>33.73976135253906</v>
       </c>
       <c r="G78" t="n">
         <v>2114000</v>
@@ -2238,7 +2238,7 @@
         <v>41.79999923706055</v>
       </c>
       <c r="F81" t="n">
-        <v>41.71316528320312</v>
+        <v>41.71316146850586</v>
       </c>
       <c r="G81" t="n">
         <v>3499100</v>
@@ -2307,7 +2307,7 @@
         <v>41.34999847412109</v>
       </c>
       <c r="F84" t="n">
-        <v>41.26410293579102</v>
+        <v>41.26410675048828</v>
       </c>
       <c r="G84" t="n">
         <v>3097400</v>
@@ -2353,7 +2353,7 @@
         <v>38.7599983215332</v>
       </c>
       <c r="F86" t="n">
-        <v>38.67947769165039</v>
+        <v>38.67948150634766</v>
       </c>
       <c r="G86" t="n">
         <v>2483600</v>
@@ -2376,7 +2376,7 @@
         <v>36.16999816894531</v>
       </c>
       <c r="F87" t="n">
-        <v>36.09485626220703</v>
+        <v>36.0948600769043</v>
       </c>
       <c r="G87" t="n">
         <v>3135100</v>
@@ -2399,7 +2399,7 @@
         <v>33.79000091552734</v>
       </c>
       <c r="F88" t="n">
-        <v>33.71980667114258</v>
+        <v>33.71980285644531</v>
       </c>
       <c r="G88" t="n">
         <v>2492500</v>
@@ -2445,7 +2445,7 @@
         <v>33.36000061035156</v>
       </c>
       <c r="F90" t="n">
-        <v>33.29069900512695</v>
+        <v>33.29070281982422</v>
       </c>
       <c r="G90" t="n">
         <v>2412300</v>
@@ -2525,7 +2525,7 @@
         <v>24.5</v>
       </c>
       <c r="F94" t="n">
-        <v>24.45713424682617</v>
+        <v>24.4571361541748</v>
       </c>
       <c r="G94" t="n">
         <v>3405200</v>
@@ -2548,7 +2548,7 @@
         <v>28.93000030517578</v>
       </c>
       <c r="F95" t="n">
-        <v>28.8793830871582</v>
+        <v>28.87938499450684</v>
       </c>
       <c r="G95" t="n">
         <v>2421800</v>
@@ -2571,7 +2571,7 @@
         <v>27.90999984741211</v>
       </c>
       <c r="F96" t="n">
-        <v>27.86116981506348</v>
+        <v>27.86116790771484</v>
       </c>
       <c r="G96" t="n">
         <v>1663400</v>
@@ -2640,7 +2640,7 @@
         <v>27.19000053405762</v>
       </c>
       <c r="F99" t="n">
-        <v>27.14242744445801</v>
+        <v>27.14242935180664</v>
       </c>
       <c r="G99" t="n">
         <v>3205000</v>
@@ -2663,7 +2663,7 @@
         <v>29.04999923706055</v>
       </c>
       <c r="F100" t="n">
-        <v>28.99917221069336</v>
+        <v>28.99917030334473</v>
       </c>
       <c r="G100" t="n">
         <v>3090400</v>
@@ -2686,7 +2686,7 @@
         <v>30.29000091552734</v>
       </c>
       <c r="F101" t="n">
-        <v>30.23700523376465</v>
+        <v>30.23700332641602</v>
       </c>
       <c r="G101" t="n">
         <v>3419100</v>
@@ -2709,7 +2709,7 @@
         <v>31.54000091552734</v>
       </c>
       <c r="F102" t="n">
-        <v>31.48481941223145</v>
+        <v>31.48481750488281</v>
       </c>
       <c r="G102" t="n">
         <v>1670000</v>
@@ -2755,7 +2755,7 @@
         <v>26.01000022888184</v>
       </c>
       <c r="F104" t="n">
-        <v>25.96449279785156</v>
+        <v>25.96449089050293</v>
       </c>
       <c r="G104" t="n">
         <v>4950800</v>
@@ -2858,7 +2858,7 @@
         <v>24.13999938964844</v>
       </c>
       <c r="F109" t="n">
-        <v>24.10663414001465</v>
+        <v>24.10663223266602</v>
       </c>
       <c r="G109" t="n">
         <v>1581200</v>
@@ -2973,7 +2973,7 @@
         <v>22.30999946594238</v>
       </c>
       <c r="F114" t="n">
-        <v>22.27916145324707</v>
+        <v>22.2791633605957</v>
       </c>
       <c r="G114" t="n">
         <v>1336400</v>
@@ -3019,7 +3019,7 @@
         <v>27.35000038146973</v>
       </c>
       <c r="F116" t="n">
-        <v>27.31219673156738</v>
+        <v>27.31219482421875</v>
       </c>
       <c r="G116" t="n">
         <v>1510600</v>
@@ -3065,7 +3065,7 @@
         <v>26.45000076293945</v>
       </c>
       <c r="F118" t="n">
-        <v>26.4134407043457</v>
+        <v>26.41344261169434</v>
       </c>
       <c r="G118" t="n">
         <v>1862100</v>

</xml_diff>